<commit_message>
Git segir enn að eigi eftir að commit-a en BÚINN AÐ ÞVÍ
</commit_message>
<xml_diff>
--- a/VefHopVerk1_Checklist.xlsx
+++ b/VefHopVerk1_Checklist.xlsx
@@ -8,18 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugmeistarinn\Documents\VefHop1\Hopverkefni1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0350D558-76B6-4A6B-9619-7DF946126838}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BE072C-A61D-4BA4-B1EB-5F6D7FAA3BDB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7020" xr2:uid="{44854158-C567-4FAB-A8D3-C3C818E52A72}"/>
   </bookViews>
   <sheets>
-    <sheet name="ToDo" sheetId="3" r:id="rId1"/>
-    <sheet name="Gefin fyrirmæli" sheetId="1" r:id="rId2"/>
-    <sheet name="Mat" sheetId="2" r:id="rId3"/>
+    <sheet name="STATUS (Heild)" sheetId="5" r:id="rId1"/>
+    <sheet name="HEADER" sheetId="7" r:id="rId2"/>
+    <sheet name="FOOTER" sheetId="6" r:id="rId3"/>
+    <sheet name="index" sheetId="9" r:id="rId4"/>
+    <sheet name="staff" sheetId="8" r:id="rId5"/>
+    <sheet name="products" sheetId="10" r:id="rId6"/>
+    <sheet name="cart" sheetId="3" r:id="rId7"/>
+    <sheet name="#Gefin fyrirmæli" sheetId="1" r:id="rId8"/>
+    <sheet name="Mat" sheetId="2" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Gefin fyrirmæli'!$E$1:$H$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ToDo!$E$1:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'#Gefin fyrirmæli'!$E$1:$H$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">cart!$E$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FOOTER!$E$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">HEADER!$E$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">index!$E$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">products!$E$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">staff!$E$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STATUS (Heild)'!$E$1:$H$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,6 +43,354 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hugmeistarinn</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{ACCA5D56-8031-47AC-AC18-1915F90D183F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Telur fjölda atriða sem byrjað er á. (Miðað við það sem sett er inn í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{60069CB4-7CBF-40DA-803C-CD14B3CEF7FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Þetta reiknar heildarframgang í verkefninu. (Miðað við að sett sé inn %-lokið í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hugmeistarinn</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{736D8AA0-69FD-4986-B80C-76C3D8996620}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Telur fjölda atriða sem byrjað er á. (Miðað við það sem sett er inn í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{9A7D6017-41D5-4378-BFCB-064BE59A62C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Þetta reiknar heildarframgang í verkefninu. (Miðað við að sett sé inn %-lokið í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hugmeistarinn</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{EBFB1CFD-658C-45CC-844D-8775F13FAC3C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Telur fjölda atriða sem byrjað er á. (Miðað við það sem sett er inn í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{FFC2E4F4-55FF-498B-A2C8-7A7E2613350E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Þetta reiknar heildarframgang í verkefninu. (Miðað við að sett sé inn %-lokið í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hugmeistarinn</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{070DE068-D578-469F-9494-184FB45154F4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Telur fjölda atriða sem byrjað er á. (Miðað við það sem sett er inn í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{DF72D9CF-2A62-479C-9D98-0C5A07396DFD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Þetta reiknar heildarframgang í verkefninu. (Miðað við að sett sé inn %-lokið í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hugmeistarinn</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{0E00A5D0-82B2-4A58-AADF-75137B8012A2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Telur fjölda atriða sem byrjað er á. (Miðað við það sem sett er inn í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{037BFB27-25F5-461A-8628-DB620A7F956A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Þetta reiknar heildarframgang í verkefninu. (Miðað við að sett sé inn %-lokið í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hugmeistarinn</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{2AC4CF70-7F3A-457D-A65F-2251B2EDD1FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Telur fjölda atriða sem byrjað er á. (Miðað við það sem sett er inn í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{D2D20BEB-02B8-4529-9CA1-F3A751C87356}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hugmeistarinn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Þetta reiknar heildarframgang í verkefninu. (Miðað við að sett sé inn %-lokið í dálk H)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hugmeistarinn</author>
@@ -88,7 +448,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hugmeistarinn</author>
@@ -171,7 +531,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="123">
   <si>
     <t>Útlit</t>
   </si>
@@ -499,12 +859,6 @@
     <t>COPYRIGHT: Neðst í miðju: "(copyright icon) 2018 Vöruhúsið"</t>
   </si>
   <si>
-    <t>FYRIRSAGNIR: Rétt stærð, litur (SVARTUR) og letur (Oswald, Verdana eða serif).</t>
-  </si>
-  <si>
-    <t>Rétt letur (Oswald, Verdana eða serif) á Titli og navigation.</t>
-  </si>
-  <si>
     <t>LITUR: Réttur backgroundcolor (#000000, #ffffff, #afb281, #cee8ff, #fcffd2 og #cc9694.) stærð HEADERs</t>
   </si>
   <si>
@@ -520,7 +874,55 @@
     <t>TEXTI: rétt letur ( Open Sans eða helvetica, arial eða sans-serif) &amp; Stærð.</t>
   </si>
   <si>
-    <t>VERÐ: fyrir vörur, rétt letur &amp; Stærð.</t>
+    <t>Forsíða</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>Skjal tilbúið?</t>
+  </si>
+  <si>
+    <t>index.html &amp; styles.scss</t>
+  </si>
+  <si>
+    <t>staff.html</t>
+  </si>
+  <si>
+    <t>cart.html</t>
+  </si>
+  <si>
+    <t>Vöruflokkar í fæti skulu allir vísa á pages/products.html.</t>
+  </si>
+  <si>
+    <t>FYRIRSAGNIR</t>
+  </si>
+  <si>
+    <t>TEXTI (meginmál)</t>
+  </si>
+  <si>
+    <t>Karfa</t>
+  </si>
+  <si>
+    <t>Vörur</t>
+  </si>
+  <si>
+    <t>cart.html &amp; styles.scss</t>
+  </si>
+  <si>
+    <t>products.html &amp; styles.scss</t>
+  </si>
+  <si>
+    <t>staff.html &amp; styles.scss</t>
+  </si>
+  <si>
+    <t>.scss</t>
+  </si>
+  <si>
+    <t>BEM</t>
+  </si>
+  <si>
+    <t>HTML skjal notað BEM fyrir ÖLL NÖFN.</t>
   </si>
 </sst>
 </file>
@@ -530,7 +932,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +1015,28 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -715,7 +1139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -785,6 +1209,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1100,12 +1533,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22CBC58-7D5F-4487-A9E2-579C9B4C97E5}">
-  <dimension ref="A1:K55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CEF6A6-4F76-495E-99CB-0840DDE516C5}">
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,607 +1557,215 @@
         <v>4</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>57</v>
       </c>
       <c r="G1" s="6" t="str">
-        <f>CONCATENATE("TO-DOs - Smt: ",COUNTA(G2:G102)," atriði")</f>
-        <v>TO-DOs - Smt: 41 atriði</v>
+        <f>CONCATENATE("STATUS Verkefnis -  Smt: ",COUNTA(G2:G63)," atriði")</f>
+        <v>STATUS Verkefnis -  Smt: 11 atriði</v>
       </c>
       <c r="H1" s="12" t="str">
-        <f>CONCATENATE("Byrjað á ",COUNTA(H2:H102)," atriðum")</f>
-        <v>Byrjað á 0 atriðum</v>
+        <f>CONCATENATE("Byrjað á ",COUNTA(H2:H63)," atriðum")</f>
+        <v>Byrjað á 6 atriðum</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>70</v>
       </c>
       <c r="K1" s="22">
-        <f>SUM(H2:H102) / COUNTA(G2:G102)</f>
+        <f>SUM(H2:H63) / COUNTA(G2:G63)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="16" t="s">
-        <v>7</v>
+    <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="27">
+        <f>HEADER!K1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="27">
+        <f>FOOTER!K1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="27">
+        <f>index!K3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="26" t="s">
+        <v>107</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="16" t="s">
-        <v>7</v>
+        <v>119</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="27">
+        <f>staff!K1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="26" t="s">
+        <v>116</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="20"/>
-    </row>
-    <row r="7" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="16" t="s">
-        <v>7</v>
+        <v>118</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="27">
+        <f>products!K1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="26" t="s">
+        <v>115</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="27">
+        <f>cart!K1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="16" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="16"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G8" s="5" t="str">
+        <f>"-  README.md skrá skal vera í rót verkefnis.
+-  Upplýsingar um hvernig keyra skuli verkefnið
+- Lýsingu á uppsetningu verkefnis, hvernig því er skipt í möppur, hvernig CSS er skipulagt og fleira sem á við
+- Upplýsingar um alla sem unnu verkefni"</f>
+        <v>-  README.md skrá skal vera í rót verkefnis.
+-  Upplýsingar um hvernig keyra skuli verkefnið
+- Lýsingu á uppsetningu verkefnis, hvernig því er skipt í möppur, hvernig CSS er skipulagt og fleira sem á við
+- Upplýsingar um alla sem unnu verkefni</v>
+      </c>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="J9"/>
+      <c r="K9"/>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
       <c r="E10" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>85</v>
+        <v>32</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="J10"/>
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
       <c r="E11" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>85</v>
+        <v>32</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="19"/>
-    </row>
-    <row r="12" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="J11"/>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
       <c r="E12" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="5:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="5:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E18" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="5:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="5:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20" s="19"/>
-    </row>
-    <row r="21" spans="5:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H21" s="19"/>
-    </row>
-    <row r="22" spans="5:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H22" s="19"/>
-    </row>
-    <row r="23" spans="5:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="E23" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H23" s="19"/>
-    </row>
-    <row r="24" spans="5:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="E24" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H24" s="19"/>
-    </row>
-    <row r="25" spans="5:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="E25" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H25" s="19"/>
-    </row>
-    <row r="26" spans="5:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="E26" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="14" t="str">
-        <f>"= Fyrirmynd í 1500px"</f>
-        <v>= Fyrirmynd í 1500px</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H26" s="19"/>
-    </row>
-    <row r="27" spans="5:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="E27" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="14" t="str">
-        <f>"= Fyrirmynd í 800px"</f>
-        <v>= Fyrirmynd í 800px</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H27" s="19"/>
-    </row>
-    <row r="28" spans="5:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="E28" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="14" t="str">
-        <f>"= Fyrirmynd í 500px"</f>
-        <v>= Fyrirmynd í 500px</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H28" s="19"/>
-    </row>
-    <row r="29" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="19"/>
-    </row>
-    <row r="30" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H30" s="19"/>
-    </row>
-    <row r="31" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H31" s="19"/>
-    </row>
-    <row r="32" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E32" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H32" s="19"/>
-    </row>
-    <row r="33" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H33" s="19"/>
-    </row>
-    <row r="34" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E34" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H34" s="19"/>
-    </row>
-    <row r="35" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E35" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H35" s="19"/>
-    </row>
-    <row r="36" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E36" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H36" s="19"/>
-    </row>
-    <row r="37" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E37" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H37" s="19"/>
-    </row>
-    <row r="38" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E38" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H38" s="19"/>
-    </row>
-    <row r="39" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E39" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H39" s="19"/>
-    </row>
-    <row r="40" spans="5:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="E40" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F40" s="14" t="str">
-        <f>"= Fyrirmynd í 1500px"</f>
-        <v>= Fyrirmynd í 1500px</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H40" s="19"/>
-    </row>
-    <row r="41" spans="5:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41" s="14" t="str">
-        <f>"= Fyrirmynd í 800px"</f>
-        <v>= Fyrirmynd í 800px</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H41" s="19"/>
-    </row>
-    <row r="42" spans="5:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="E42" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="14" t="str">
-        <f>"= Fyrirmynd í 500px"</f>
-        <v>= Fyrirmynd í 500px</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H42" s="19"/>
-    </row>
-    <row r="43" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E43" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H43" s="19"/>
-    </row>
-    <row r="44" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E44" s="16"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="19"/>
-    </row>
-    <row r="45" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="16"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="19"/>
-    </row>
-    <row r="46" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E46" s="16"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="19"/>
-    </row>
-    <row r="47" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E47" s="16"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="19"/>
-    </row>
-    <row r="48" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E48" s="16"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="19"/>
-    </row>
-    <row r="49" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E49" s="16"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="19"/>
-    </row>
-    <row r="50" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="16"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="19"/>
-    </row>
-    <row r="51" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E51" s="16"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="19"/>
-    </row>
-    <row r="52" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E52" s="16"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="19"/>
-    </row>
-    <row r="53" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E53" s="16"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="19"/>
-    </row>
-    <row r="54" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E54" s="16"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="19"/>
-    </row>
-    <row r="55" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E55" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="19"/>
+        <v>52</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="5" t="str">
+        <f>"- Nöfn allra í hóp ásamt notendanafni
+- Slóð á GitHub repo fyrir verkefni, og dæmatímakennara boðið
+- Slóð á verkefnið keyrandi á vefnum"</f>
+        <v>- Nöfn allra í hóp ásamt notendanafni
+- Slóð á GitHub repo fyrir verkefni, og dæmatímakennara boðið
+- Slóð á verkefnið keyrandi á vefnum</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="J12"/>
+      <c r="K12"/>
     </row>
   </sheetData>
-  <autoFilter ref="E1:H10" xr:uid="{4D074974-705E-4536-ACEA-E2BDBACDAE8B}"/>
+  <autoFilter ref="E1:H12" xr:uid="{4D074974-705E-4536-ACEA-E2BDBACDAE8B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1732,12 +1773,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03469A41-EF83-4F17-9C63-75BED0816D7F}">
-  <dimension ref="A1:K37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DE74A9-C5CE-41F7-9CB5-0E997B4F5620}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,6 +1797,1584 @@
         <v>4</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="6" t="str">
+        <f>CONCATENATE("TO-DOs - Smt: ",COUNTA(G2:G54)," atriði")</f>
+        <v>TO-DOs - Smt: 13 atriði</v>
+      </c>
+      <c r="H1" s="12" t="str">
+        <f>CONCATENATE("Byrjað á ",COUNTA(H2:H54)," atriðum")</f>
+        <v>Byrjað á 0 atriðum</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="22">
+        <f>SUM(H2:H54) / COUNTA(G2:G54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="5" t="str">
+        <f>"- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60."</f>
+        <v>- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60.</v>
+      </c>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E11" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E12" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="5" t="str">
+        <f>"- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter."</f>
+        <v>- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter.</v>
+      </c>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E13" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E14" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="E1:H1" xr:uid="{4D074974-705E-4536-ACEA-E2BDBACDAE8B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925FAD3A-C50F-46CD-B3FB-D07ABD6AB18A}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="24.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="6" t="str">
+        <f>CONCATENATE("TO-DOs - Smt: ",COUNTA(G2:G52)," atriði")</f>
+        <v>TO-DOs - Smt: 11 atriði</v>
+      </c>
+      <c r="H1" s="12" t="str">
+        <f>CONCATENATE("Byrjað á ",COUNTA(H2:H52)," atriðum")</f>
+        <v>Byrjað á 0 atriðum</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="22">
+        <f>SUM(H2:H52) / COUNTA(G2:G52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="J2"/>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="J3"/>
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="J4"/>
+      <c r="K4"/>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="J5"/>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E6" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E7" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="5" t="str">
+        <f>"- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60."</f>
+        <v>- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60.</v>
+      </c>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E8" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E9" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E10" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="5" t="str">
+        <f>"- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter."</f>
+        <v>- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter.</v>
+      </c>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E11" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="20"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="E1:H1" xr:uid="{4D074974-705E-4536-ACEA-E2BDBACDAE8B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C475A3-5B71-4F18-BD26-94E16022F808}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="24.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="6" t="str">
+        <f>CONCATENATE("TO-DOs - Smt: ",COUNTA(G2:G52)," atriði")</f>
+        <v>TO-DOs - Smt: 15 atriði</v>
+      </c>
+      <c r="H1" s="12" t="str">
+        <f>CONCATENATE("Byrjað á ",COUNTA(H2:H52)," atriðum")</f>
+        <v>Byrjað á 0 atriðum</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="22">
+        <f>SUM(H2:H52) / COUNTA(G2:G52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="14" t="str">
+        <f>"= Fyrirmynd í 1500px"</f>
+        <v>= Fyrirmynd í 1500px</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="14" t="str">
+        <f>"= Fyrirmynd í 800px"</f>
+        <v>= Fyrirmynd í 800px</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="14" t="str">
+        <f>"= Fyrirmynd í 500px"</f>
+        <v>= Fyrirmynd í 500px</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="5" t="str">
+        <f>"- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60."</f>
+        <v>- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60.</v>
+      </c>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E14" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="5" t="str">
+        <f>"- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter."</f>
+        <v>- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter.</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E15" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E16" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="20"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="E1:H1" xr:uid="{4D074974-705E-4536-ACEA-E2BDBACDAE8B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF27FD87-3CC6-43B6-B671-358347578D3D}">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="24.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="6" t="str">
+        <f>CONCATENATE("TO-DOs - Smt: ",COUNTA(G2:G73)," atriði")</f>
+        <v>TO-DOs - Smt: 18 atriði</v>
+      </c>
+      <c r="H1" s="12" t="str">
+        <f>CONCATENATE("Byrjað á ",COUNTA(H2:H73)," atriðum")</f>
+        <v>Byrjað á 0 atriðum</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="22">
+        <f>SUM(H2:H73) / COUNTA(G2:G73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E4" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E5" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E6" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E7" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="14" t="str">
+        <f>"= Fyrirmynd í 1500px"</f>
+        <v>= Fyrirmynd í 1500px</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E8" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="14" t="str">
+        <f>"= Fyrirmynd í 800px"</f>
+        <v>= Fyrirmynd í 800px</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E9" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="14" t="str">
+        <f>"= Fyrirmynd í 500px"</f>
+        <v>= Fyrirmynd í 500px</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="5" t="str">
+        <f>"- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60."</f>
+        <v>- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60.</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E16" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="5" t="str">
+        <f>"- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter."</f>
+        <v>- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter.</v>
+      </c>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="16"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21" spans="5:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="E21" s="16"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="5:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="E22" s="16"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="5:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="E23" s="16"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="19"/>
+    </row>
+    <row r="24" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="16"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="16"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="16"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="19"/>
+    </row>
+    <row r="27" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="16"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="19"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="E1:H1" xr:uid="{4D074974-705E-4536-ACEA-E2BDBACDAE8B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEC5136-C194-4C97-9096-7355F41103EE}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="24.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="6" t="str">
+        <f>CONCATENATE("TO-DOs - Smt: ",COUNTA(G2:G62)," atriði")</f>
+        <v>TO-DOs - Smt: 19 atriði</v>
+      </c>
+      <c r="H1" s="12" t="str">
+        <f>CONCATENATE("Byrjað á ",COUNTA(H2:H62)," atriðum")</f>
+        <v>Byrjað á 0 atriðum</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="22">
+        <f>SUM(H2:H62) / COUNTA(G2:G62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E5" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E6" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E7" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="14" t="str">
+        <f>"= Fyrirmynd í 1500px"</f>
+        <v>= Fyrirmynd í 1500px</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E8" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="14" t="str">
+        <f>"= Fyrirmynd í 800px"</f>
+        <v>= Fyrirmynd í 800px</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E9" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="14" t="str">
+        <f>"= Fyrirmynd í 500px"</f>
+        <v>= Fyrirmynd í 500px</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="5" t="str">
+        <f>"- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60."</f>
+        <v>- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60.</v>
+      </c>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="5" t="str">
+        <f>"- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter."</f>
+        <v>- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter.</v>
+      </c>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="5:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="E20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="20"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="E1:H1" xr:uid="{4D074974-705E-4536-ACEA-E2BDBACDAE8B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22CBC58-7D5F-4487-A9E2-579C9B4C97E5}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="24.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="6" t="str">
+        <f>CONCATENATE("TO-DOs - Smt: ",COUNTA(G2:G67)," atriði")</f>
+        <v>TO-DOs - Smt: 16 atriði</v>
+      </c>
+      <c r="H1" s="12" t="str">
+        <f>CONCATENATE("Byrjað á ",COUNTA(H2:H67)," atriðum")</f>
+        <v>Byrjað á 0 atriðum</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="22">
+        <f>SUM(H2:H67) / COUNTA(G2:G67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E4" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E5" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="E6" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="14" t="str">
+        <f>"= Fyrirmynd í 1500px"</f>
+        <v>= Fyrirmynd í 1500px</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E8" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="14" t="str">
+        <f>"= Fyrirmynd í 800px"</f>
+        <v>= Fyrirmynd í 800px</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="E9" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="14" t="str">
+        <f>"= Fyrirmynd í 500px"</f>
+        <v>= Fyrirmynd í 500px</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="5" t="str">
+        <f>"- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60."</f>
+        <v>- Grunn leturstærð er 16px og fylgja allar aðrar leturgerðir eftirfarandi skala:                                  
+12 14 16 18 21 24 36 48 60.</v>
+      </c>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="5" t="str">
+        <f>"- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter."</f>
+        <v>- Flest allt er sett upp í 12 dálka grind með 20px gutter.
+- Öll bil eru hálft, heilt, tvöfalt eða þrefalt margfeldi af gutter.</v>
+      </c>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="16"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="16"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="16"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="16"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="5:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="16"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="19"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="E1:H1" xr:uid="{4D074974-705E-4536-ACEA-E2BDBACDAE8B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03469A41-EF83-4F17-9C63-75BED0816D7F}">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="24.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>65</v>
       </c>
       <c r="F1" s="7" t="s">
@@ -2224,7 +3843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16169417-04B1-4B65-BF46-F7BDC93C05D8}">
   <dimension ref="G1:H9"/>
   <sheetViews>

</xml_diff>